<commit_message>
add get_sales function to grab sales orders data
</commit_message>
<xml_diff>
--- a/unleashed_v3/unl_enquiry/20180408_unl_test.xlsx
+++ b/unleashed_v3/unl_enquiry/20180408_unl_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>Product Code</t>
   </si>
@@ -25,31 +25,310 @@
     <t>Quantity On Hand</t>
   </si>
   <si>
-    <t>Quantity On Purchase</t>
-  </si>
-  <si>
-    <t>PPPRAS</t>
-  </si>
-  <si>
-    <t>BXPCPRTRKT</t>
-  </si>
-  <si>
-    <t>BXPCPRMN2ML</t>
-  </si>
-  <si>
-    <t>INPULLULAN</t>
-  </si>
-  <si>
-    <t>Partial Bulk Pro Accelerator S</t>
-  </si>
-  <si>
-    <t>Box ProCell Pro Aftercare Serums Sample Set</t>
-  </si>
-  <si>
-    <t>Box ProCell Pro Microneedling Solution 2ml</t>
-  </si>
-  <si>
-    <t>Ingredient Pullulan</t>
+    <t>Quantity On Sales</t>
+  </si>
+  <si>
+    <t>AAMDSAKT</t>
+  </si>
+  <si>
+    <t>AAMDAC30ML</t>
+  </si>
+  <si>
+    <t>BXAAMDAC30ML</t>
+  </si>
+  <si>
+    <t>FBAAMDAC30ML</t>
+  </si>
+  <si>
+    <t>EBAAMDAC30ML</t>
+  </si>
+  <si>
+    <t>FBMDACYW30ML</t>
+  </si>
+  <si>
+    <t>EBINYW30ML</t>
+  </si>
+  <si>
+    <t>EBPMYW30ML</t>
+  </si>
+  <si>
+    <t>FLMDACYW30ML</t>
+  </si>
+  <si>
+    <t>INSCCM</t>
+  </si>
+  <si>
+    <t>AAMDSE30ML</t>
+  </si>
+  <si>
+    <t>BXAAMDSE30ML</t>
+  </si>
+  <si>
+    <t>FBAAMDSE30ML</t>
+  </si>
+  <si>
+    <t>EBAAMDSE30ML</t>
+  </si>
+  <si>
+    <t>FBMDSEYW30ML</t>
+  </si>
+  <si>
+    <t>FLMDSEYW30ML</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>AAPRSAKT</t>
+  </si>
+  <si>
+    <t>AAPRAC30ML</t>
+  </si>
+  <si>
+    <t>BXAAPRAC30ML</t>
+  </si>
+  <si>
+    <t>FBAAPRAC30ML</t>
+  </si>
+  <si>
+    <t>EBAAPRAC30ML</t>
+  </si>
+  <si>
+    <t>FBPRACYW30ML</t>
+  </si>
+  <si>
+    <t>FLPRACYW30ML</t>
+  </si>
+  <si>
+    <t>AAPRSE30ML</t>
+  </si>
+  <si>
+    <t>BXAAPRSE30ML</t>
+  </si>
+  <si>
+    <t>FBAAPRSE30ML</t>
+  </si>
+  <si>
+    <t>EBAAPRSE30ML</t>
+  </si>
+  <si>
+    <t>FBPRSEYW30ML</t>
+  </si>
+  <si>
+    <t>FLPRSEYW30ML</t>
+  </si>
+  <si>
+    <t>AACL120ML</t>
+  </si>
+  <si>
+    <t>FBAACL120ML</t>
+  </si>
+  <si>
+    <t>FPAACL</t>
+  </si>
+  <si>
+    <t>EBAACL120ML</t>
+  </si>
+  <si>
+    <t>BXAACL120ML</t>
+  </si>
+  <si>
+    <t>AAMDMNBX</t>
+  </si>
+  <si>
+    <t>BXAAMDMN</t>
+  </si>
+  <si>
+    <t>FBAAMDMN2ML</t>
+  </si>
+  <si>
+    <t>FBMDMN2ML</t>
+  </si>
+  <si>
+    <t>EBMN2ML</t>
+  </si>
+  <si>
+    <t>FPMDMN</t>
+  </si>
+  <si>
+    <t>STAAMDMN2ML</t>
+  </si>
+  <si>
+    <t>AAMDVRBX</t>
+  </si>
+  <si>
+    <t>BXAAMDVR</t>
+  </si>
+  <si>
+    <t>FBAAMDVR4ML</t>
+  </si>
+  <si>
+    <t>EBAAMDVR4MLSB</t>
+  </si>
+  <si>
+    <t>EBAAMDVR4ML</t>
+  </si>
+  <si>
+    <t>SBVR4ML</t>
+  </si>
+  <si>
+    <t>FLAAMDVR4ML</t>
+  </si>
+  <si>
+    <t>BXAAMDVRIS</t>
+  </si>
+  <si>
+    <t>BXAAMDVRSL</t>
+  </si>
+  <si>
+    <t>AnteAGE MD System</t>
+  </si>
+  <si>
+    <t>AnteAGE MD Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Box AnteAGE MD Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE MD Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE MD Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle MD Accelerator 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>Bottle Inner 30ml PKG/YW</t>
+  </si>
+  <si>
+    <t>Bottle Pump 30ml PKG/YW</t>
+  </si>
+  <si>
+    <t>Fill MD Accelerator 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>Ingredient Stem Cell Conditioned Media</t>
+  </si>
+  <si>
+    <t>AnteAGE MD Serum 30ml</t>
+  </si>
+  <si>
+    <t>Box AnteAGE MD Serum 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE MD Serum 30ml</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE MD Serum 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle MD Serum 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>Fill MD Serum 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>AnteAGE System</t>
+  </si>
+  <si>
+    <t>AnteAGE Pro Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Box AnteAGE Pro Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE Pro Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE Pro Accelerator 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle Pro Accelerator 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>Fill Pro Accelerator 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>AnteAGE Pro Serum 30ml</t>
+  </si>
+  <si>
+    <t>Box AnteAGE Pro Serum 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE Pro Serum 30ml</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE Pro Serum 30ml</t>
+  </si>
+  <si>
+    <t>Final Bottle Pro Serum 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>Fill Pro Serum 30ml YonWoo</t>
+  </si>
+  <si>
+    <t>AnteAGE Cleanser Retail 120ml</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE Cleanser Retail 120ml</t>
+  </si>
+  <si>
+    <t>Finished Bulk AnteAGE Cleanser</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE Cleanser Crimp Tube 120ml</t>
+  </si>
+  <si>
+    <t>Box AnteAGE Cleanser Retail 120ml</t>
+  </si>
+  <si>
+    <t>AnteAGE MD Microneedling Solution Box (5)</t>
+  </si>
+  <si>
+    <t>Box AnteAGE MD Microneedling (5)</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE MD Microneedling Solution 2ml</t>
+  </si>
+  <si>
+    <t>Final Bottle MD Microneedling Solution 2ml</t>
+  </si>
+  <si>
+    <t>Bottle Microneedling Solution Roller 2ml</t>
+  </si>
+  <si>
+    <t>Finished Bulk MD Microneedling Solution</t>
+  </si>
+  <si>
+    <t>Sticker AnteAGE MD Microneedling Solution 2ml</t>
+  </si>
+  <si>
+    <t>AnteAGE MD VRS Box (6)</t>
+  </si>
+  <si>
+    <t>Box AnteAGE MD VRS (6)</t>
+  </si>
+  <si>
+    <t>Final Bottle AnteAGE MD VRS 4ml</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE MD VRS 4ml Shrink Band</t>
+  </si>
+  <si>
+    <t>Bottle AnteAGE MD VRS 4ml</t>
+  </si>
+  <si>
+    <t>Shrink Band VRS 4ml</t>
+  </si>
+  <si>
+    <t>Fill AnteAGE MD VRS 4ml</t>
+  </si>
+  <si>
+    <t>Box AnteAGE MD VRS (6) - Insert</t>
+  </si>
+  <si>
+    <t>Box AnteAGE MD VRS (6) - Sleeve</t>
   </si>
 </sst>
 </file>
@@ -407,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,10 +711,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>111</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -443,13 +725,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C3">
-        <v>5392</v>
+        <v>256</v>
       </c>
       <c r="D3">
-        <v>2500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,13 +739,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C4">
-        <v>1450</v>
+        <v>2590</v>
       </c>
       <c r="D4">
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -471,10 +753,793 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>5926</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>576</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>40430</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9">
+        <v>11054</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>54.7605</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>1059</v>
+      </c>
+      <c r="D12">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13">
+        <v>1666</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15">
+        <v>4110</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <v>40430</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18">
+        <v>11054</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>54.7605</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23">
+        <v>613</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24">
+        <v>1982</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>5165</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27">
+        <v>38</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28">
+        <v>40430</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29">
+        <v>11054</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31">
+        <v>54.7605</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32">
+        <v>610</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33">
+        <v>2018</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35">
+        <v>5000</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37">
+        <v>40430</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38">
+        <v>11054</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40">
+        <v>54.7605</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42">
+        <v>203</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44">
+        <v>45.0208</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45">
+        <v>2369</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46">
+        <v>2545</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48">
+        <v>483</v>
+      </c>
+      <c r="D48">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49">
+        <v>3171</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50">
+        <v>126</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51">
+        <v>2870</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52">
+        <v>29778.2897</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54">
+        <v>12963</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58">
+        <v>210</v>
+      </c>
+      <c r="D58">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59">
+        <v>210</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" t="s">
         <v>100</v>
+      </c>
+      <c r="C60">
+        <v>332</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61">
+        <v>27593</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added both order quantity options
</commit_message>
<xml_diff>
--- a/unleashed_v3/unl_enquiry/20180408_unl_test.xlsx
+++ b/unleashed_v3/unl_enquiry/20180408_unl_test.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_Repos\unleashed\unleashed_v3\unl_enquiry\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D8CF33AC-8D1B-4F08-892F-37645EEF2C14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t>Product Code</t>
   </si>
@@ -26,6 +32,9 @@
   </si>
   <si>
     <t>Quantity On Sales</t>
+  </si>
+  <si>
+    <t>Quantity On Purchase</t>
   </si>
   <si>
     <t>AAMDSAKT</t>
@@ -334,8 +343,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +407,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -444,7 +461,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -476,9 +493,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -510,6 +545,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -685,14 +738,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,13 +766,16 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -719,13 +783,16 @@
       <c r="D2">
         <v>181</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>256</v>
@@ -733,13 +800,16 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>2590</v>
@@ -747,13 +817,16 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -761,13 +834,16 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>5926</v>
@@ -775,13 +851,16 @@
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>576</v>
@@ -789,13 +868,16 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C8">
         <v>40430</v>
@@ -803,13 +885,16 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>11054</v>
@@ -817,13 +902,16 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>36500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -831,13 +919,16 @@
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11">
         <v>54.7605</v>
@@ -845,13 +936,16 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>1059</v>
@@ -859,13 +953,16 @@
       <c r="D12">
         <v>660</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>1666</v>
@@ -873,13 +970,16 @@
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -887,13 +987,16 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>4110</v>
@@ -901,13 +1004,16 @@
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -915,13 +1021,16 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17">
         <v>40430</v>
@@ -929,13 +1038,16 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>11054</v>
@@ -943,13 +1055,16 @@
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>36500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -957,13 +1072,16 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20">
         <v>54.7605</v>
@@ -971,18 +1089,21 @@
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -990,13 +1111,16 @@
       <c r="D22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>613</v>
@@ -1004,13 +1128,16 @@
       <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C24">
         <v>1982</v>
@@ -1018,13 +1145,16 @@
       <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1032,13 +1162,16 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>5165</v>
@@ -1046,13 +1179,16 @@
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27">
         <v>38</v>
@@ -1060,13 +1196,16 @@
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>40430</v>
@@ -1074,13 +1213,16 @@
       <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29">
         <v>11054</v>
@@ -1088,13 +1230,16 @@
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>36500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1102,13 +1247,16 @@
       <c r="D30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C31">
         <v>54.7605</v>
@@ -1116,13 +1264,16 @@
       <c r="D31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C32">
         <v>610</v>
@@ -1130,13 +1281,16 @@
       <c r="D32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C33">
         <v>2018</v>
@@ -1144,13 +1298,16 @@
       <c r="D33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1158,13 +1315,16 @@
       <c r="D34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C35">
         <v>5000</v>
@@ -1172,13 +1332,16 @@
       <c r="D35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1186,13 +1349,16 @@
       <c r="D36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C37">
         <v>40430</v>
@@ -1200,13 +1366,16 @@
       <c r="D37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C38">
         <v>11054</v>
@@ -1214,13 +1383,16 @@
       <c r="D38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>36500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1228,13 +1400,16 @@
       <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C40">
         <v>54.7605</v>
@@ -1242,18 +1417,21 @@
       <c r="D40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42">
         <v>203</v>
@@ -1261,13 +1439,16 @@
       <c r="D42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1275,27 +1456,33 @@
       <c r="D43">
         <v>145</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C44">
-        <v>45.0208</v>
+        <v>45.020800000000001</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C45">
         <v>2369</v>
@@ -1303,13 +1490,16 @@
       <c r="D45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C46">
         <v>2545</v>
@@ -1317,18 +1507,21 @@
       <c r="D46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C48">
         <v>483</v>
@@ -1336,13 +1529,16 @@
       <c r="D48">
         <v>305</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C49">
         <v>3171</v>
@@ -1350,13 +1546,16 @@
       <c r="D49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C50">
         <v>126</v>
@@ -1364,13 +1563,16 @@
       <c r="D50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C51">
         <v>2870</v>
@@ -1378,38 +1580,47 @@
       <c r="D51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C52">
-        <v>29778.2897</v>
+        <v>29778.289700000001</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C54">
         <v>12963</v>
@@ -1417,18 +1628,21 @@
       <c r="D54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1436,24 +1650,30 @@
       <c r="D56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D57">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C58">
         <v>210</v>
@@ -1461,13 +1681,16 @@
       <c r="D58">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C59">
         <v>210</v>
@@ -1475,13 +1698,16 @@
       <c r="D59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C60">
         <v>332</v>
@@ -1489,13 +1715,16 @@
       <c r="D60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C61">
         <v>27593</v>
@@ -1503,43 +1732,55 @@
       <c r="D61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>